<commit_message>
experiment D, dataset A, B, C
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cs\data mining\project2\DM_project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F00239-8C4A-4759-B8C7-EF740B79DCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47954CDC-060B-4A69-A9AB-B2518431FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -75,13 +84,13 @@
     <t>percentage split</t>
   </si>
   <si>
-    <t>A is a preprocessed dataset which missing values are imputed with mean value (for numeric) or mode value (for nominal) by using proprocess.py. For ID3, numeric data will be transformed to nominal data by using WEKA filter: weka.filters.unsupervised.attribute.NumericToNominal</t>
-  </si>
-  <si>
     <t>B is preprocessed dataset similar to A but the BandNumber and Day attributes are omitted</t>
   </si>
   <si>
     <t>C is preprocessed dataset only remains: species wing, weight, culmen, hallux, tail, standardtail, sex</t>
+  </si>
+  <si>
+    <t>A is a preprocessed dataset which missing values are imputed with mean value (for numeric) or mode value (for nominal) by using proprocess.py. Numeric data will be transformed to nominal data by using WEKA filter: weka.filters.unsupervised.attribute.NumericToNominal</t>
   </si>
 </sst>
 </file>
@@ -295,12 +304,6 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -313,10 +316,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +609,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,310 +621,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
+      <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="16" t="s">
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="16" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="2" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4">
-        <v>98.458100000000002</v>
-      </c>
-      <c r="D3" s="5">
-        <v>99.229100000000003</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="C3" s="2">
+        <v>99.5595</v>
+      </c>
+      <c r="D3" s="3">
+        <v>98.127799999999993</v>
+      </c>
+      <c r="E3" s="4">
         <v>100</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4">
-        <v>98.017600000000002</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="C4" s="2">
+        <v>95.594700000000003</v>
+      </c>
+      <c r="D4" s="3">
+        <v>93.722499999999997</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="3">
+        <v>97.985470000000007</v>
+      </c>
+      <c r="M4" s="3">
+        <v>97.841880000000003</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5">
+        <v>94.174800000000005</v>
+      </c>
+      <c r="D5" s="6">
+        <v>77.993499999999997</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
+        <v>99.339200000000005</v>
+      </c>
+      <c r="D6" s="3">
+        <v>98.127799999999993</v>
+      </c>
+      <c r="E6" s="4">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
+        <v>96.035200000000003</v>
+      </c>
+      <c r="D7" s="3">
+        <v>93.722499999999997</v>
+      </c>
+      <c r="E7" s="4">
+        <v>80.066100000000006</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="3">
+        <v>97.97448</v>
+      </c>
+      <c r="M7" s="3">
+        <v>97.841880000000003</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>94.498400000000004</v>
+      </c>
+      <c r="D8" s="6">
+        <v>77.993499999999997</v>
+      </c>
+      <c r="E8" s="7">
+        <v>84.465999999999994</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <v>99.779700000000005</v>
+      </c>
+      <c r="D9" s="3">
         <v>98.237899999999996</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="8" t="s">
+      <c r="E9" s="4">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>97.907499999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>93.722499999999997</v>
+      </c>
+      <c r="E10" s="4">
+        <v>80.176199999999994</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="3">
+        <v>97.963369999999998</v>
+      </c>
+      <c r="M10" s="3">
+        <v>98.017700000000005</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10"/>
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7">
-        <v>98.058300000000003</v>
-      </c>
-      <c r="D5" s="8">
-        <v>98.058300000000003</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4">
-        <v>99.339200000000005</v>
-      </c>
-      <c r="D6" s="5">
-        <v>98.127799999999993</v>
-      </c>
-      <c r="E6" s="6">
-        <v>100</v>
-      </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4">
-        <v>96.035200000000003</v>
-      </c>
-      <c r="D7" s="5">
-        <v>93.722499999999997</v>
-      </c>
-      <c r="E7" s="6">
-        <v>80.066100000000006</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12"/>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="7">
-        <v>94.498400000000004</v>
-      </c>
-      <c r="D8" s="8">
-        <v>77.993499999999997</v>
-      </c>
-      <c r="E8" s="9">
-        <v>84.465999999999994</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4">
-        <v>98.017600000000002</v>
-      </c>
-      <c r="D9" s="5">
-        <v>99.339200000000005</v>
-      </c>
-      <c r="E9" s="6">
-        <v>100</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4">
-        <v>97.687200000000004</v>
-      </c>
-      <c r="D10" s="5">
-        <v>98.127799999999993</v>
-      </c>
-      <c r="E10" s="6">
-        <v>80.176199999999994</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7">
-        <v>98.381900000000002</v>
-      </c>
-      <c r="D11" s="8">
-        <v>98.058300000000003</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="C11" s="5">
+        <v>96.440100000000001</v>
+      </c>
+      <c r="D11" s="6">
+        <v>92.880300000000005</v>
+      </c>
+      <c r="E11" s="7">
         <v>86.407799999999995</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>